<commit_message>
add py from my_PC
</commit_message>
<xml_diff>
--- a/other/githubのイシューで使う日付作成.xlsx
+++ b/other/githubのイシューで使う日付作成.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\81908\MyGitHub\kaggle_Cassava\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425F35B9-01B2-4EC4-AEEF-9EDD0A2E6355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A87604-34AA-4C12-9CE5-39C23F7E0B8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5925" yWindow="3930" windowWidth="16485" windowHeight="11235" activeTab="1" xr2:uid="{141D6723-FA80-4333-98C5-ACEA15F02A19}"/>
+    <workbookView xWindow="28680" yWindow="-12885" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{141D6723-FA80-4333-98C5-ACEA15F02A19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE569F3-01FF-4933-A0A2-73561C5B3C54}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -722,15 +722,15 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>20210101</v>
+        <v>20210201</v>
       </c>
       <c r="D2" t="str">
         <f>A2&amp;" "&amp;B2+10</f>
-        <v>### 20210111</v>
+        <v>### 20210211</v>
       </c>
       <c r="F2" t="str">
         <f>A2&amp;" "&amp;B2+20</f>
-        <v>### 20210121</v>
+        <v>### 20210221</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -743,11 +743,11 @@
         <v>0</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4:D29" si="0">A4</f>
+        <f t="shared" ref="D4" si="0">A4</f>
         <v>--------------------------------------------------------</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F30" si="1">A4</f>
+        <f t="shared" ref="F4" si="1">A4</f>
         <v>--------------------------------------------------------</v>
       </c>
     </row>
@@ -756,15 +756,15 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>20210102</v>
+        <v>20210202</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" ref="D5:D29" si="2">A5&amp;" "&amp;B5+10</f>
-        <v>### 20210112</v>
+        <f t="shared" ref="D5" si="2">A5&amp;" "&amp;B5+10</f>
+        <v>### 20210212</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="F5:F30" si="3">A5&amp;" "&amp;B5+20</f>
-        <v>### 20210122</v>
+        <f t="shared" ref="F5" si="3">A5&amp;" "&amp;B5+20</f>
+        <v>### 20210222</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -777,11 +777,11 @@
         <v>0</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ref="D7:D29" si="4">A7</f>
+        <f t="shared" ref="D7" si="4">A7</f>
         <v>--------------------------------------------------------</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ref="F7:F30" si="5">A7</f>
+        <f t="shared" ref="F7" si="5">A7</f>
         <v>--------------------------------------------------------</v>
       </c>
     </row>
@@ -790,15 +790,15 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>20210103</v>
+        <v>20210203</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" ref="D8:D29" si="6">A8&amp;" "&amp;B8+10</f>
-        <v>### 20210113</v>
+        <f t="shared" ref="D8" si="6">A8&amp;" "&amp;B8+10</f>
+        <v>### 20210213</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" ref="F8:F30" si="7">A8&amp;" "&amp;B8+20</f>
-        <v>### 20210123</v>
+        <f t="shared" ref="F8" si="7">A8&amp;" "&amp;B8+20</f>
+        <v>### 20210223</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -811,11 +811,11 @@
         <v>0</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" ref="D10:D29" si="8">A10</f>
+        <f t="shared" ref="D10" si="8">A10</f>
         <v>--------------------------------------------------------</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" ref="F10:F30" si="9">A10</f>
+        <f t="shared" ref="F10" si="9">A10</f>
         <v>--------------------------------------------------------</v>
       </c>
     </row>
@@ -824,15 +824,15 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>20210104</v>
+        <v>20210204</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" ref="D11:D29" si="10">A11&amp;" "&amp;B11+10</f>
-        <v>### 20210114</v>
+        <f t="shared" ref="D11" si="10">A11&amp;" "&amp;B11+10</f>
+        <v>### 20210214</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" ref="F11:F30" si="11">A11&amp;" "&amp;B11+20</f>
-        <v>### 20210124</v>
+        <f t="shared" ref="F11" si="11">A11&amp;" "&amp;B11+20</f>
+        <v>### 20210224</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
@@ -845,11 +845,11 @@
         <v>0</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" ref="D13:D29" si="12">A13</f>
+        <f t="shared" ref="D13" si="12">A13</f>
         <v>--------------------------------------------------------</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" ref="F13:F30" si="13">A13</f>
+        <f t="shared" ref="F13" si="13">A13</f>
         <v>--------------------------------------------------------</v>
       </c>
     </row>
@@ -858,15 +858,15 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>20210105</v>
+        <v>20210205</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" ref="D14:D29" si="14">A14&amp;" "&amp;B14+10</f>
-        <v>### 20210115</v>
+        <f t="shared" ref="D14" si="14">A14&amp;" "&amp;B14+10</f>
+        <v>### 20210215</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" ref="F14:F30" si="15">A14&amp;" "&amp;B14+20</f>
-        <v>### 20210125</v>
+        <f t="shared" ref="F14" si="15">A14&amp;" "&amp;B14+20</f>
+        <v>### 20210225</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
@@ -879,11 +879,11 @@
         <v>0</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" ref="D16:D29" si="16">A16</f>
+        <f t="shared" ref="D16" si="16">A16</f>
         <v>--------------------------------------------------------</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" ref="F16:F30" si="17">A16</f>
+        <f t="shared" ref="F16" si="17">A16</f>
         <v>--------------------------------------------------------</v>
       </c>
     </row>
@@ -892,15 +892,15 @@
         <v>11</v>
       </c>
       <c r="B17">
-        <v>20210106</v>
+        <v>20210206</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" ref="D17:D29" si="18">A17&amp;" "&amp;B17+10</f>
-        <v>### 20210116</v>
+        <f t="shared" ref="D17" si="18">A17&amp;" "&amp;B17+10</f>
+        <v>### 20210216</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" ref="F17:F30" si="19">A17&amp;" "&amp;B17+20</f>
-        <v>### 20210126</v>
+        <f t="shared" ref="F17" si="19">A17&amp;" "&amp;B17+20</f>
+        <v>### 20210226</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
@@ -913,11 +913,11 @@
         <v>0</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" ref="D19:D29" si="20">A19</f>
+        <f t="shared" ref="D19" si="20">A19</f>
         <v>--------------------------------------------------------</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" ref="F19:F30" si="21">A19</f>
+        <f t="shared" ref="F19" si="21">A19</f>
         <v>--------------------------------------------------------</v>
       </c>
     </row>
@@ -926,15 +926,15 @@
         <v>11</v>
       </c>
       <c r="B20">
-        <v>20210107</v>
+        <v>20210207</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" ref="D20:D29" si="22">A20&amp;" "&amp;B20+10</f>
-        <v>### 20210117</v>
+        <f t="shared" ref="D20" si="22">A20&amp;" "&amp;B20+10</f>
+        <v>### 20210217</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" ref="F20:F30" si="23">A20&amp;" "&amp;B20+20</f>
-        <v>### 20210127</v>
+        <f t="shared" ref="F20" si="23">A20&amp;" "&amp;B20+20</f>
+        <v>### 20210227</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
@@ -947,11 +947,11 @@
         <v>0</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" ref="D22:D29" si="24">A22</f>
+        <f t="shared" ref="D22" si="24">A22</f>
         <v>--------------------------------------------------------</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" ref="F22:F30" si="25">A22</f>
+        <f t="shared" ref="F22" si="25">A22</f>
         <v>--------------------------------------------------------</v>
       </c>
     </row>
@@ -960,15 +960,15 @@
         <v>11</v>
       </c>
       <c r="B23">
-        <v>20210108</v>
+        <v>20210208</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" ref="D23:D29" si="26">A23&amp;" "&amp;B23+10</f>
-        <v>### 20210118</v>
+        <f t="shared" ref="D23" si="26">A23&amp;" "&amp;B23+10</f>
+        <v>### 20210218</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" ref="F23:F30" si="27">A23&amp;" "&amp;B23+20</f>
-        <v>### 20210128</v>
+        <f t="shared" ref="F23" si="27">A23&amp;" "&amp;B23+20</f>
+        <v>### 20210228</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
@@ -981,11 +981,11 @@
         <v>0</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" ref="D25:D29" si="28">A25</f>
+        <f t="shared" ref="D25" si="28">A25</f>
         <v>--------------------------------------------------------</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" ref="F25:F30" si="29">A25</f>
+        <f t="shared" ref="F25" si="29">A25</f>
         <v>--------------------------------------------------------</v>
       </c>
     </row>
@@ -994,15 +994,15 @@
         <v>11</v>
       </c>
       <c r="B26">
-        <v>20210109</v>
+        <v>20210209</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" ref="D26:D29" si="30">A26&amp;" "&amp;B26+10</f>
-        <v>### 20210119</v>
+        <f t="shared" ref="D26" si="30">A26&amp;" "&amp;B26+10</f>
+        <v>### 20210219</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" ref="F26:F30" si="31">A26&amp;" "&amp;B26+20</f>
-        <v>### 20210129</v>
+        <f t="shared" ref="F26" si="31">A26&amp;" "&amp;B26+20</f>
+        <v>### 20210229</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
@@ -1010,11 +1010,11 @@
         <v>0</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" ref="D28:D29" si="32">A28</f>
+        <f t="shared" ref="D28" si="32">A28</f>
         <v>--------------------------------------------------------</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" ref="F28:F30" si="33">A28</f>
+        <f t="shared" ref="F28" si="33">A28</f>
         <v>--------------------------------------------------------</v>
       </c>
     </row>
@@ -1023,15 +1023,15 @@
         <v>11</v>
       </c>
       <c r="B29">
-        <v>20210110</v>
+        <v>20210210</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" ref="D29" si="34">A29&amp;" "&amp;B29+10</f>
-        <v>### 20210120</v>
+        <v>### 20210220</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" ref="F29:F30" si="35">A29&amp;" "&amp;B29+20</f>
-        <v>### 20210130</v>
+        <f t="shared" ref="F29" si="35">A29&amp;" "&amp;B29+20</f>
+        <v>### 20210230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>